<commit_message>
New unit tests check phyloseq_from_JSON
</commit_message>
<xml_diff>
--- a/inst/extdata/dummyData/Dummy_User_Mapfile.xlsx
+++ b/inst/extdata/dummyData/Dummy_User_Mapfile.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Kit ID</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>dummydata</t>
+  </si>
+  <si>
+    <t>dummy original</t>
   </si>
 </sst>
 </file>
@@ -157,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -167,6 +170,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,6 +510,26 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9">
+        <v>42587</v>
+      </c>
+      <c r="D3">
+        <v>75519</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>